<commit_message>
Various improvements, fixes. Closes #8
LargeMojiDisp is now able to clicked
PreferenceActivity with header on XLargeScreen devices
Saving last search kanji (in defaultSharedPreferences)
Start search on hardkeyboard's enter key pressed
Implements Browse on click preference
Added Show_Toasts preference
Added "search queue" feature
</commit_message>
<xml_diff>
--- a/01-設計書/設計書.xlsx
+++ b/01-設計書/設計書.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="画面設計書" sheetId="2" r:id="rId1"/>
@@ -101,38 +101,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="AE12" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="ＭＳ Ｐゴシック"/>
-            <family val="3"/>
-            <charset val="128"/>
-          </rPr>
-          <t>作成者:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="ＭＳ Ｐゴシック"/>
-            <family val="3"/>
-            <charset val="128"/>
-          </rPr>
-          <t xml:space="preserve">
-Copy</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="131">
   <si>
     <t>Input search</t>
     <phoneticPr fontId="5"/>
@@ -767,10 +741,6 @@
     <phoneticPr fontId="4"/>
   </si>
   <si>
-    <t>P</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
     <t>http://developer.android.com/guide/topics/manifest/uses-sdk-element.html</t>
   </si>
   <si>
@@ -842,6 +812,40 @@
   </si>
   <si>
     <t>http://developer.android.com/guide/components/intents-filters.html</t>
+  </si>
+  <si>
+    <t>http://commons.wikimedia.org/wiki/Commons:Chinese_characters_decomposition</t>
+  </si>
+  <si>
+    <t>wikimedia commons</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>http://www.yellowbridge.com/chinese/character-etymology.php?zi=%E7%89%A2</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>https://code.google.com/p/cjklib/wiki/DatabaseScheme</t>
+  </si>
+  <si>
+    <t>Interesting Project in Python</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>入力した漢字を全部ここに入れる</t>
+    <rPh sb="0" eb="2">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>カンジ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>ゼンブ</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>イ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
   </si>
 </sst>
 </file>
@@ -987,12 +991,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Wingdings"/>
-      <charset val="2"/>
-    </font>
-    <font>
       <strike/>
       <sz val="11"/>
       <color theme="1"/>
@@ -1011,6 +1009,13 @@
       <color theme="1"/>
       <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1039,7 +1044,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="48">
+  <borders count="50">
     <border>
       <left/>
       <right/>
@@ -1606,6 +1611,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1614,7 +1645,7 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1">
       <alignment vertical="center"/>
@@ -1778,13 +1809,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1796,7 +1821,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1810,7 +1835,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="47" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1880,10 +1909,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="48" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="47" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="49" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="34" xfId="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="35" xfId="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="ハイパーリンク" xfId="2" builtinId="8"/>
@@ -1915,7 +1954,7 @@
     <xdr:to>
       <xdr:col>64</xdr:col>
       <xdr:colOff>10886</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>54429</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1961,13 +2000,13 @@
     <xdr:from>
       <xdr:col>62</xdr:col>
       <xdr:colOff>21770</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>54429</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>64</xdr:col>
       <xdr:colOff>21771</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>54429</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2013,13 +2052,13 @@
     <xdr:from>
       <xdr:col>62</xdr:col>
       <xdr:colOff>32655</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>54429</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>64</xdr:col>
       <xdr:colOff>32656</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>87085</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2123,7 +2162,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>10885</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2635,10 +2674,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D2:CQ54"/>
+  <dimension ref="D2:CQ55"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AF7" sqref="AF7"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -2666,35 +2705,35 @@
     </row>
     <row r="5" spans="4:95" ht="13.8" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="4:95" ht="19.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G6" s="70" t="s">
+      <c r="G6" s="68" t="s">
+        <v>111</v>
+      </c>
+      <c r="H6" s="67"/>
+      <c r="I6" s="67"/>
+      <c r="J6" s="67"/>
+      <c r="K6" s="67"/>
+      <c r="L6" s="67"/>
+      <c r="M6" s="67"/>
+      <c r="N6" s="67"/>
+      <c r="O6" s="67"/>
+      <c r="P6" s="67"/>
+      <c r="Q6" s="67"/>
+      <c r="R6" s="67"/>
+      <c r="S6" s="67"/>
+      <c r="T6" s="67"/>
+      <c r="U6" s="67"/>
+      <c r="V6" s="67"/>
+      <c r="W6" s="67"/>
+      <c r="X6" s="67"/>
+      <c r="Y6" s="67"/>
+      <c r="Z6" s="67"/>
+      <c r="AA6" s="67"/>
+      <c r="AB6" s="67"/>
+      <c r="AC6" s="67"/>
+      <c r="AD6" s="67"/>
+      <c r="AE6" s="67"/>
+      <c r="AF6" s="69" t="s">
         <v>112</v>
-      </c>
-      <c r="H6" s="69"/>
-      <c r="I6" s="69"/>
-      <c r="J6" s="69"/>
-      <c r="K6" s="69"/>
-      <c r="L6" s="69"/>
-      <c r="M6" s="69"/>
-      <c r="N6" s="69"/>
-      <c r="O6" s="69"/>
-      <c r="P6" s="69"/>
-      <c r="Q6" s="69"/>
-      <c r="R6" s="69"/>
-      <c r="S6" s="69"/>
-      <c r="T6" s="69"/>
-      <c r="U6" s="69"/>
-      <c r="V6" s="69"/>
-      <c r="W6" s="69"/>
-      <c r="X6" s="69"/>
-      <c r="Y6" s="69"/>
-      <c r="Z6" s="69"/>
-      <c r="AA6" s="69"/>
-      <c r="AB6" s="69"/>
-      <c r="AC6" s="69"/>
-      <c r="AD6" s="69"/>
-      <c r="AE6" s="69"/>
-      <c r="AF6" s="71" t="s">
-        <v>113</v>
       </c>
       <c r="AG6" s="5"/>
       <c r="AH6" s="5"/>
@@ -3006,45 +3045,38 @@
       <c r="BE10" s="5"/>
       <c r="BF10" s="5"/>
       <c r="BG10" s="5"/>
-      <c r="BH10" s="5">
-        <v>6</v>
-      </c>
+      <c r="BH10" s="5"/>
       <c r="BI10" s="5"/>
       <c r="BJ10" s="7"/>
-      <c r="BS10" s="36" t="s">
-        <v>35</v>
-      </c>
-      <c r="BW10" s="36" t="s">
-        <v>40</v>
-      </c>
+      <c r="BS10" s="36"/>
+      <c r="BW10" s="36"/>
     </row>
     <row r="11" spans="4:95" x14ac:dyDescent="0.2">
       <c r="G11" s="6"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="O11" s="5"/>
-      <c r="P11" s="5"/>
-      <c r="Q11" s="5"/>
-      <c r="R11" s="5"/>
-      <c r="S11" s="5"/>
-      <c r="T11" s="5"/>
-      <c r="U11" s="5"/>
-      <c r="V11" s="5"/>
-      <c r="W11" s="5"/>
-      <c r="X11" s="5"/>
-      <c r="Y11" s="5"/>
-      <c r="Z11" s="5"/>
-      <c r="AA11" s="5"/>
-      <c r="AB11" s="5"/>
+      <c r="H11" s="108" t="s">
+        <v>130</v>
+      </c>
+      <c r="I11" s="106"/>
+      <c r="J11" s="106"/>
+      <c r="K11" s="106"/>
+      <c r="L11" s="106"/>
+      <c r="M11" s="106"/>
+      <c r="N11" s="106"/>
+      <c r="O11" s="106"/>
+      <c r="P11" s="106"/>
+      <c r="Q11" s="106"/>
+      <c r="R11" s="106"/>
+      <c r="S11" s="106"/>
+      <c r="T11" s="106"/>
+      <c r="U11" s="106"/>
+      <c r="V11" s="106"/>
+      <c r="W11" s="106"/>
+      <c r="X11" s="106"/>
+      <c r="Y11" s="106"/>
+      <c r="Z11" s="106"/>
+      <c r="AA11" s="106"/>
+      <c r="AB11" s="107"/>
       <c r="AC11" s="5"/>
-      <c r="AD11" s="5"/>
       <c r="AE11" s="5"/>
       <c r="AF11" s="7"/>
       <c r="AG11" s="5"/>
@@ -3052,19 +3084,13 @@
       <c r="AI11" s="5"/>
       <c r="AJ11" s="5"/>
       <c r="AK11" s="6"/>
-      <c r="AL11" s="31" t="s">
-        <v>15</v>
-      </c>
+      <c r="AL11" s="5"/>
       <c r="AM11" s="5"/>
       <c r="AN11" s="5"/>
       <c r="AO11" s="5"/>
       <c r="AP11" s="5"/>
-      <c r="AQ11" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="AR11" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="AQ11" s="5"/>
+      <c r="AR11" s="5"/>
       <c r="AS11" s="5"/>
       <c r="AT11" s="5"/>
       <c r="AU11" s="5"/>
@@ -3080,136 +3106,153 @@
       <c r="BE11" s="5"/>
       <c r="BF11" s="5"/>
       <c r="BG11" s="5"/>
-      <c r="BH11" s="5"/>
+      <c r="BH11" s="5">
+        <v>6</v>
+      </c>
       <c r="BI11" s="5"/>
       <c r="BJ11" s="7"/>
-    </row>
-    <row r="12" spans="4:95" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BS11" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="BW11" s="36" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="4:95" x14ac:dyDescent="0.2">
       <c r="G12" s="6"/>
-      <c r="H12" s="8">
-        <v>2</v>
-      </c>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="10"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
       <c r="M12" s="5"/>
-      <c r="N12" s="8">
+      <c r="N12" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="O12" s="9"/>
-      <c r="P12" s="9"/>
-      <c r="Q12" s="9"/>
-      <c r="R12" s="9"/>
-      <c r="S12" s="9"/>
-      <c r="T12" s="9"/>
-      <c r="U12" s="9"/>
-      <c r="V12" s="9"/>
-      <c r="W12" s="9"/>
-      <c r="X12" s="9"/>
-      <c r="Y12" s="9"/>
-      <c r="Z12" s="9"/>
-      <c r="AA12" s="9"/>
-      <c r="AB12" s="9"/>
-      <c r="AC12" s="14">
-        <v>5</v>
-      </c>
-      <c r="AE12" s="66">
-        <v>4</v>
-      </c>
+      <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="5"/>
+      <c r="S12" s="5"/>
+      <c r="T12" s="5"/>
+      <c r="U12" s="5"/>
+      <c r="V12" s="5"/>
+      <c r="W12" s="5"/>
+      <c r="X12" s="5"/>
+      <c r="Y12" s="5"/>
+      <c r="Z12" s="5"/>
+      <c r="AA12" s="5"/>
+      <c r="AB12" s="5"/>
+      <c r="AC12" s="5"/>
+      <c r="AD12" s="5"/>
+      <c r="AE12" s="5"/>
       <c r="AF12" s="7"/>
       <c r="AG12" s="5"/>
       <c r="AH12" s="5"/>
       <c r="AI12" s="5"/>
       <c r="AJ12" s="5"/>
       <c r="AK12" s="6"/>
-      <c r="AL12" s="84" t="s">
-        <v>14</v>
-      </c>
-      <c r="AM12" s="85"/>
-      <c r="AN12" s="85"/>
-      <c r="AO12" s="85"/>
-      <c r="AP12" s="86"/>
-      <c r="AQ12" s="5"/>
-      <c r="AR12" s="8"/>
-      <c r="AS12" s="9"/>
-      <c r="AT12" s="9"/>
-      <c r="AU12" s="9"/>
-      <c r="AV12" s="9"/>
-      <c r="AW12" s="9"/>
-      <c r="AX12" s="9"/>
-      <c r="AY12" s="9"/>
-      <c r="AZ12" s="9"/>
-      <c r="BA12" s="9"/>
-      <c r="BB12" s="9"/>
-      <c r="BC12" s="9"/>
-      <c r="BD12" s="9"/>
-      <c r="BE12" s="9"/>
-      <c r="BF12" s="9"/>
-      <c r="BG12" s="9"/>
-      <c r="BH12" s="9"/>
-      <c r="BI12" s="14">
+      <c r="AL12" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="AM12" s="5"/>
+      <c r="AN12" s="5"/>
+      <c r="AO12" s="5"/>
+      <c r="AP12" s="5"/>
+      <c r="AQ12" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="AR12" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AS12" s="5"/>
+      <c r="AT12" s="5"/>
+      <c r="AU12" s="5"/>
+      <c r="AV12" s="5"/>
+      <c r="AW12" s="5"/>
+      <c r="AX12" s="5"/>
+      <c r="AY12" s="5"/>
+      <c r="AZ12" s="5"/>
+      <c r="BA12" s="5"/>
+      <c r="BB12" s="5"/>
+      <c r="BC12" s="5"/>
+      <c r="BD12" s="5"/>
+      <c r="BE12" s="5"/>
+      <c r="BF12" s="5"/>
+      <c r="BG12" s="5"/>
+      <c r="BH12" s="5"/>
+      <c r="BI12" s="5"/>
+      <c r="BJ12" s="7"/>
+    </row>
+    <row r="13" spans="4:95" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G13" s="6"/>
+      <c r="H13" s="8">
+        <v>2</v>
+      </c>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="8">
+        <v>3</v>
+      </c>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="9"/>
+      <c r="S13" s="9"/>
+      <c r="T13" s="9"/>
+      <c r="U13" s="9"/>
+      <c r="V13" s="9"/>
+      <c r="W13" s="9"/>
+      <c r="X13" s="9"/>
+      <c r="Y13" s="9"/>
+      <c r="Z13" s="9"/>
+      <c r="AA13" s="9"/>
+      <c r="AB13" s="9"/>
+      <c r="AC13" s="9"/>
+      <c r="AD13" s="9"/>
+      <c r="AE13" s="14">
         <v>5</v>
       </c>
-      <c r="BJ12" s="7"/>
-    </row>
-    <row r="13" spans="4:95" x14ac:dyDescent="0.2">
-      <c r="G13" s="6"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="16"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="15"/>
-      <c r="O13" s="5"/>
-      <c r="P13" s="5"/>
-      <c r="Q13" s="5"/>
-      <c r="R13" s="5"/>
-      <c r="S13" s="5"/>
-      <c r="T13" s="5"/>
-      <c r="U13" s="5"/>
-      <c r="V13" s="5"/>
-      <c r="W13" s="5"/>
-      <c r="X13" s="5"/>
-      <c r="Y13" s="5"/>
-      <c r="Z13" s="5"/>
-      <c r="AA13" s="5"/>
-      <c r="AB13" s="5"/>
-      <c r="AC13" s="17"/>
       <c r="AF13" s="7"/>
       <c r="AG13" s="5"/>
       <c r="AH13" s="5"/>
       <c r="AI13" s="5"/>
       <c r="AJ13" s="5"/>
       <c r="AK13" s="6"/>
-      <c r="AL13" s="87"/>
-      <c r="AM13" s="88"/>
-      <c r="AN13" s="88"/>
-      <c r="AO13" s="88"/>
-      <c r="AP13" s="89"/>
+      <c r="AL13" s="84" t="s">
+        <v>14</v>
+      </c>
+      <c r="AM13" s="85"/>
+      <c r="AN13" s="85"/>
+      <c r="AO13" s="85"/>
+      <c r="AP13" s="86"/>
       <c r="AQ13" s="5"/>
-      <c r="AR13" s="15"/>
-      <c r="AS13" s="5"/>
-      <c r="AT13" s="5"/>
-      <c r="AU13" s="5"/>
-      <c r="AV13" s="5"/>
-      <c r="AW13" s="5"/>
-      <c r="AX13" s="5"/>
-      <c r="AY13" s="5"/>
-      <c r="AZ13" s="5"/>
-      <c r="BA13" s="5"/>
-      <c r="BB13" s="5"/>
-      <c r="BC13" s="5"/>
-      <c r="BD13" s="5"/>
-      <c r="BE13" s="5"/>
-      <c r="BF13" s="5"/>
-      <c r="BG13" s="5"/>
-      <c r="BH13" s="5"/>
-      <c r="BI13" s="17"/>
+      <c r="AR13" s="8"/>
+      <c r="AS13" s="9"/>
+      <c r="AT13" s="9"/>
+      <c r="AU13" s="9"/>
+      <c r="AV13" s="9"/>
+      <c r="AW13" s="9"/>
+      <c r="AX13" s="9"/>
+      <c r="AY13" s="9"/>
+      <c r="AZ13" s="9"/>
+      <c r="BA13" s="9"/>
+      <c r="BB13" s="9"/>
+      <c r="BC13" s="9"/>
+      <c r="BD13" s="9"/>
+      <c r="BE13" s="9"/>
+      <c r="BF13" s="9"/>
+      <c r="BG13" s="9"/>
+      <c r="BH13" s="9"/>
+      <c r="BI13" s="14">
+        <v>5</v>
+      </c>
       <c r="BJ13" s="7"/>
     </row>
-    <row r="14" spans="4:95" ht="13.2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="4:95" x14ac:dyDescent="0.2">
       <c r="G14" s="6"/>
       <c r="H14" s="15"/>
       <c r="I14" s="5"/>
@@ -3232,10 +3275,9 @@
       <c r="Z14" s="5"/>
       <c r="AA14" s="5"/>
       <c r="AB14" s="5"/>
-      <c r="AC14" s="17"/>
-      <c r="AE14" s="65" t="s">
-        <v>108</v>
-      </c>
+      <c r="AC14" s="5"/>
+      <c r="AD14" s="5"/>
+      <c r="AE14" s="17"/>
       <c r="AF14" s="7"/>
       <c r="AG14" s="5"/>
       <c r="AH14" s="5"/>
@@ -3267,40 +3309,8 @@
       <c r="BH14" s="5"/>
       <c r="BI14" s="17"/>
       <c r="BJ14" s="7"/>
-      <c r="BN14" s="36" t="s">
-        <v>31</v>
-      </c>
-      <c r="BS14" s="8"/>
-      <c r="BT14" s="9"/>
-      <c r="BU14" s="9"/>
-      <c r="BV14" s="9"/>
-      <c r="BW14" s="10"/>
-      <c r="BX14" s="5"/>
-      <c r="BY14" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="BZ14" s="40"/>
-      <c r="CA14" s="40"/>
-      <c r="CB14" s="40"/>
-      <c r="CC14" s="40"/>
-      <c r="CD14" s="40"/>
-      <c r="CE14" s="40"/>
-      <c r="CF14" s="40"/>
-      <c r="CG14" s="40"/>
-      <c r="CH14" s="40"/>
-      <c r="CI14" s="40"/>
-      <c r="CJ14" s="40"/>
-      <c r="CK14" s="40"/>
-      <c r="CL14" s="40"/>
-      <c r="CM14" s="40"/>
-      <c r="CN14" s="40"/>
-      <c r="CO14" s="40"/>
-      <c r="CP14" s="41"/>
-    </row>
-    <row r="15" spans="4:95" x14ac:dyDescent="0.2">
-      <c r="D15" s="37" t="s">
-        <v>37</v>
-      </c>
+    </row>
+    <row r="15" spans="4:95" ht="13.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G15" s="6"/>
       <c r="H15" s="15"/>
       <c r="I15" s="5"/>
@@ -3323,7 +3333,9 @@
       <c r="Z15" s="5"/>
       <c r="AA15" s="5"/>
       <c r="AB15" s="5"/>
-      <c r="AC15" s="17"/>
+      <c r="AC15" s="5"/>
+      <c r="AD15" s="5"/>
+      <c r="AE15" s="17"/>
       <c r="AF15" s="7"/>
       <c r="AG15" s="5"/>
       <c r="AH15" s="5"/>
@@ -3355,173 +3367,183 @@
       <c r="BH15" s="5"/>
       <c r="BI15" s="17"/>
       <c r="BJ15" s="7"/>
-      <c r="BS15" s="15">
-        <v>2</v>
-      </c>
-      <c r="BT15" s="5"/>
-      <c r="BU15" s="5"/>
-      <c r="BV15" s="5"/>
-      <c r="BW15" s="16"/>
+      <c r="BN15" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="BS15" s="8"/>
+      <c r="BT15" s="9"/>
+      <c r="BU15" s="9"/>
+      <c r="BV15" s="9"/>
+      <c r="BW15" s="10"/>
       <c r="BX15" s="5"/>
-      <c r="BY15" s="8">
+      <c r="BY15" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="BZ15" s="9"/>
-      <c r="CA15" s="9"/>
-      <c r="CB15" s="9"/>
-      <c r="CC15" s="9"/>
-      <c r="CD15" s="9"/>
-      <c r="CE15" s="9"/>
-      <c r="CF15" s="9"/>
-      <c r="CG15" s="9"/>
-      <c r="CH15" s="9"/>
-      <c r="CI15" s="9"/>
-      <c r="CJ15" s="9"/>
-      <c r="CK15" s="9"/>
-      <c r="CL15" s="9"/>
-      <c r="CM15" s="9"/>
-      <c r="CN15" s="9"/>
-      <c r="CO15" s="9"/>
-      <c r="CP15" s="14">
-        <v>5</v>
-      </c>
+      <c r="BZ15" s="40"/>
+      <c r="CA15" s="40"/>
+      <c r="CB15" s="40"/>
+      <c r="CC15" s="40"/>
+      <c r="CD15" s="40"/>
+      <c r="CE15" s="40"/>
+      <c r="CF15" s="40"/>
+      <c r="CG15" s="40"/>
+      <c r="CH15" s="40"/>
+      <c r="CI15" s="40"/>
+      <c r="CJ15" s="40"/>
+      <c r="CK15" s="40"/>
+      <c r="CL15" s="40"/>
+      <c r="CM15" s="40"/>
+      <c r="CN15" s="40"/>
+      <c r="CO15" s="40"/>
+      <c r="CP15" s="41"/>
     </row>
     <row r="16" spans="4:95" x14ac:dyDescent="0.2">
+      <c r="D16" s="37" t="s">
+        <v>37</v>
+      </c>
       <c r="G16" s="6"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="13"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="16"/>
       <c r="M16" s="5"/>
-      <c r="N16" s="11"/>
-      <c r="O16" s="12"/>
-      <c r="P16" s="12"/>
-      <c r="Q16" s="12"/>
-      <c r="R16" s="12"/>
-      <c r="S16" s="12"/>
-      <c r="T16" s="12"/>
-      <c r="U16" s="12"/>
-      <c r="V16" s="12"/>
-      <c r="W16" s="12"/>
-      <c r="X16" s="12"/>
-      <c r="Y16" s="12"/>
-      <c r="Z16" s="12"/>
-      <c r="AA16" s="12"/>
-      <c r="AB16" s="12"/>
-      <c r="AC16" s="18"/>
+      <c r="N16" s="15"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="5"/>
+      <c r="R16" s="5"/>
+      <c r="S16" s="5"/>
+      <c r="T16" s="5"/>
+      <c r="U16" s="5"/>
+      <c r="V16" s="5"/>
+      <c r="W16" s="5"/>
+      <c r="X16" s="5"/>
+      <c r="Y16" s="5"/>
+      <c r="Z16" s="5"/>
+      <c r="AA16" s="5"/>
+      <c r="AB16" s="5"/>
+      <c r="AC16" s="5"/>
+      <c r="AD16" s="5"/>
+      <c r="AE16" s="17"/>
       <c r="AF16" s="7"/>
       <c r="AG16" s="5"/>
       <c r="AH16" s="5"/>
       <c r="AI16" s="5"/>
       <c r="AJ16" s="5"/>
       <c r="AK16" s="6"/>
-      <c r="AL16" s="90"/>
-      <c r="AM16" s="91"/>
-      <c r="AN16" s="91"/>
-      <c r="AO16" s="91"/>
-      <c r="AP16" s="92"/>
+      <c r="AL16" s="87"/>
+      <c r="AM16" s="88"/>
+      <c r="AN16" s="88"/>
+      <c r="AO16" s="88"/>
+      <c r="AP16" s="89"/>
       <c r="AQ16" s="5"/>
-      <c r="AR16" s="11"/>
-      <c r="AS16" s="12"/>
-      <c r="AT16" s="12"/>
-      <c r="AU16" s="12"/>
-      <c r="AV16" s="12"/>
-      <c r="AW16" s="12"/>
-      <c r="AX16" s="12"/>
-      <c r="AY16" s="12"/>
-      <c r="AZ16" s="12"/>
-      <c r="BA16" s="12"/>
-      <c r="BB16" s="12"/>
-      <c r="BC16" s="12"/>
-      <c r="BD16" s="12"/>
-      <c r="BE16" s="12"/>
-      <c r="BF16" s="12"/>
-      <c r="BG16" s="12"/>
-      <c r="BH16" s="12"/>
-      <c r="BI16" s="18"/>
+      <c r="AR16" s="15"/>
+      <c r="AS16" s="5"/>
+      <c r="AT16" s="5"/>
+      <c r="AU16" s="5"/>
+      <c r="AV16" s="5"/>
+      <c r="AW16" s="5"/>
+      <c r="AX16" s="5"/>
+      <c r="AY16" s="5"/>
+      <c r="AZ16" s="5"/>
+      <c r="BA16" s="5"/>
+      <c r="BB16" s="5"/>
+      <c r="BC16" s="5"/>
+      <c r="BD16" s="5"/>
+      <c r="BE16" s="5"/>
+      <c r="BF16" s="5"/>
+      <c r="BG16" s="5"/>
+      <c r="BH16" s="5"/>
+      <c r="BI16" s="17"/>
       <c r="BJ16" s="7"/>
-      <c r="BS16" s="15"/>
+      <c r="BS16" s="15">
+        <v>2</v>
+      </c>
       <c r="BT16" s="5"/>
       <c r="BU16" s="5"/>
       <c r="BV16" s="5"/>
       <c r="BW16" s="16"/>
       <c r="BX16" s="5"/>
-      <c r="BY16" s="15"/>
-      <c r="BZ16" s="5"/>
-      <c r="CA16" s="5"/>
-      <c r="CB16" s="5"/>
-      <c r="CC16" s="5"/>
-      <c r="CD16" s="5"/>
-      <c r="CE16" s="5"/>
-      <c r="CF16" s="5"/>
-      <c r="CG16" s="5"/>
-      <c r="CH16" s="5"/>
-      <c r="CI16" s="5"/>
-      <c r="CJ16" s="5"/>
-      <c r="CK16" s="5"/>
-      <c r="CL16" s="5"/>
-      <c r="CM16" s="5"/>
-      <c r="CN16" s="5"/>
-      <c r="CO16" s="5"/>
-      <c r="CP16" s="17"/>
+      <c r="BY16" s="8">
+        <v>3</v>
+      </c>
+      <c r="BZ16" s="9"/>
+      <c r="CA16" s="9"/>
+      <c r="CB16" s="9"/>
+      <c r="CC16" s="9"/>
+      <c r="CD16" s="9"/>
+      <c r="CE16" s="9"/>
+      <c r="CF16" s="9"/>
+      <c r="CG16" s="9"/>
+      <c r="CH16" s="9"/>
+      <c r="CI16" s="9"/>
+      <c r="CJ16" s="9"/>
+      <c r="CK16" s="9"/>
+      <c r="CL16" s="9"/>
+      <c r="CM16" s="9"/>
+      <c r="CN16" s="9"/>
+      <c r="CO16" s="9"/>
+      <c r="CP16" s="14">
+        <v>5</v>
+      </c>
     </row>
     <row r="17" spans="7:94" x14ac:dyDescent="0.2">
       <c r="G17" s="6"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="13"/>
       <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5"/>
-      <c r="P17" s="5"/>
-      <c r="Q17" s="5"/>
-      <c r="R17" s="5"/>
-      <c r="S17" s="5"/>
-      <c r="T17" s="5"/>
-      <c r="U17" s="5"/>
-      <c r="V17" s="5"/>
-      <c r="W17" s="5"/>
-      <c r="X17" s="5"/>
-      <c r="Y17" s="5"/>
-      <c r="Z17" s="5"/>
-      <c r="AA17" s="5"/>
-      <c r="AB17" s="5"/>
-      <c r="AC17" s="5"/>
-      <c r="AD17" s="5"/>
-      <c r="AE17" s="5"/>
+      <c r="N17" s="11"/>
+      <c r="O17" s="12"/>
+      <c r="P17" s="12"/>
+      <c r="Q17" s="12"/>
+      <c r="R17" s="12"/>
+      <c r="S17" s="12"/>
+      <c r="T17" s="12"/>
+      <c r="U17" s="12"/>
+      <c r="V17" s="12"/>
+      <c r="W17" s="12"/>
+      <c r="X17" s="12"/>
+      <c r="Y17" s="12"/>
+      <c r="Z17" s="12"/>
+      <c r="AA17" s="12"/>
+      <c r="AB17" s="12"/>
+      <c r="AC17" s="12"/>
+      <c r="AD17" s="12"/>
+      <c r="AE17" s="18"/>
       <c r="AF17" s="7"/>
       <c r="AG17" s="5"/>
       <c r="AH17" s="5"/>
       <c r="AI17" s="5"/>
       <c r="AJ17" s="5"/>
       <c r="AK17" s="6"/>
-      <c r="AL17" s="5"/>
-      <c r="AM17" s="5"/>
-      <c r="AN17" s="5"/>
-      <c r="AO17" s="5"/>
-      <c r="AP17" s="5"/>
+      <c r="AL17" s="90"/>
+      <c r="AM17" s="91"/>
+      <c r="AN17" s="91"/>
+      <c r="AO17" s="91"/>
+      <c r="AP17" s="92"/>
       <c r="AQ17" s="5"/>
-      <c r="AR17" s="5"/>
-      <c r="AS17" s="5"/>
-      <c r="AT17" s="5"/>
-      <c r="AU17" s="5"/>
-      <c r="AV17" s="5"/>
-      <c r="AW17" s="5"/>
-      <c r="AX17" s="5"/>
-      <c r="AY17" s="5"/>
-      <c r="AZ17" s="5"/>
-      <c r="BA17" s="5"/>
-      <c r="BB17" s="5"/>
-      <c r="BC17" s="5"/>
-      <c r="BD17" s="5"/>
-      <c r="BE17" s="5"/>
-      <c r="BF17" s="5"/>
-      <c r="BG17" s="5"/>
-      <c r="BH17" s="5"/>
-      <c r="BI17" s="5"/>
+      <c r="AR17" s="11"/>
+      <c r="AS17" s="12"/>
+      <c r="AT17" s="12"/>
+      <c r="AU17" s="12"/>
+      <c r="AV17" s="12"/>
+      <c r="AW17" s="12"/>
+      <c r="AX17" s="12"/>
+      <c r="AY17" s="12"/>
+      <c r="AZ17" s="12"/>
+      <c r="BA17" s="12"/>
+      <c r="BB17" s="12"/>
+      <c r="BC17" s="12"/>
+      <c r="BD17" s="12"/>
+      <c r="BE17" s="12"/>
+      <c r="BF17" s="12"/>
+      <c r="BG17" s="12"/>
+      <c r="BH17" s="12"/>
+      <c r="BI17" s="18"/>
       <c r="BJ17" s="7"/>
       <c r="BS17" s="15"/>
       <c r="BT17" s="5"/>
@@ -3550,9 +3572,7 @@
     </row>
     <row r="18" spans="7:94" x14ac:dyDescent="0.2">
       <c r="G18" s="6"/>
-      <c r="H18" s="5" t="s">
-        <v>4</v>
-      </c>
+      <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
@@ -3582,9 +3602,7 @@
       <c r="AI18" s="5"/>
       <c r="AJ18" s="5"/>
       <c r="AK18" s="6"/>
-      <c r="AL18" s="5" t="s">
-        <v>4</v>
-      </c>
+      <c r="AL18" s="5"/>
       <c r="AM18" s="5"/>
       <c r="AN18" s="5"/>
       <c r="AO18" s="5"/>
@@ -3636,151 +3654,179 @@
     </row>
     <row r="19" spans="7:94" x14ac:dyDescent="0.2">
       <c r="G19" s="6"/>
-      <c r="H19" s="8">
+      <c r="H19" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="9"/>
-      <c r="N19" s="9"/>
-      <c r="O19" s="9"/>
-      <c r="P19" s="9"/>
-      <c r="Q19" s="9"/>
-      <c r="R19" s="9"/>
-      <c r="S19" s="9"/>
-      <c r="T19" s="9"/>
-      <c r="U19" s="9"/>
-      <c r="V19" s="9"/>
-      <c r="W19" s="9"/>
-      <c r="X19" s="9"/>
-      <c r="Y19" s="9"/>
-      <c r="Z19" s="9"/>
-      <c r="AA19" s="9"/>
-      <c r="AB19" s="9"/>
-      <c r="AC19" s="9"/>
-      <c r="AD19" s="9"/>
-      <c r="AE19" s="14">
-        <v>5</v>
-      </c>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="5"/>
+      <c r="R19" s="5"/>
+      <c r="S19" s="5"/>
+      <c r="T19" s="5"/>
+      <c r="U19" s="5"/>
+      <c r="V19" s="5"/>
+      <c r="W19" s="5"/>
+      <c r="X19" s="5"/>
+      <c r="Y19" s="5"/>
+      <c r="Z19" s="5"/>
+      <c r="AA19" s="5"/>
+      <c r="AB19" s="5"/>
+      <c r="AC19" s="5"/>
+      <c r="AD19" s="5"/>
+      <c r="AE19" s="5"/>
       <c r="AF19" s="7"/>
       <c r="AG19" s="5"/>
       <c r="AH19" s="5"/>
       <c r="AI19" s="5"/>
       <c r="AJ19" s="5"/>
       <c r="AK19" s="6"/>
-      <c r="AL19" s="8">
+      <c r="AL19" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="AM19" s="9"/>
-      <c r="AN19" s="9"/>
-      <c r="AO19" s="9"/>
-      <c r="AP19" s="9"/>
-      <c r="AQ19" s="9"/>
-      <c r="AR19" s="9"/>
-      <c r="AS19" s="9"/>
-      <c r="AT19" s="9"/>
-      <c r="AU19" s="9"/>
-      <c r="AV19" s="9"/>
-      <c r="AW19" s="9"/>
-      <c r="AX19" s="9"/>
-      <c r="AY19" s="9"/>
-      <c r="AZ19" s="9"/>
-      <c r="BA19" s="9"/>
-      <c r="BB19" s="9"/>
-      <c r="BC19" s="9"/>
-      <c r="BD19" s="9"/>
-      <c r="BE19" s="9"/>
-      <c r="BF19" s="9"/>
-      <c r="BG19" s="9"/>
-      <c r="BH19" s="9"/>
-      <c r="BI19" s="14">
-        <v>5</v>
-      </c>
+      <c r="AM19" s="5"/>
+      <c r="AN19" s="5"/>
+      <c r="AO19" s="5"/>
+      <c r="AP19" s="5"/>
+      <c r="AQ19" s="5"/>
+      <c r="AR19" s="5"/>
+      <c r="AS19" s="5"/>
+      <c r="AT19" s="5"/>
+      <c r="AU19" s="5"/>
+      <c r="AV19" s="5"/>
+      <c r="AW19" s="5"/>
+      <c r="AX19" s="5"/>
+      <c r="AY19" s="5"/>
+      <c r="AZ19" s="5"/>
+      <c r="BA19" s="5"/>
+      <c r="BB19" s="5"/>
+      <c r="BC19" s="5"/>
+      <c r="BD19" s="5"/>
+      <c r="BE19" s="5"/>
+      <c r="BF19" s="5"/>
+      <c r="BG19" s="5"/>
+      <c r="BH19" s="5"/>
+      <c r="BI19" s="5"/>
       <c r="BJ19" s="7"/>
-      <c r="BS19" s="11"/>
-      <c r="BT19" s="12"/>
-      <c r="BU19" s="12"/>
-      <c r="BV19" s="12"/>
-      <c r="BW19" s="13"/>
+      <c r="BS19" s="15"/>
+      <c r="BT19" s="5"/>
+      <c r="BU19" s="5"/>
+      <c r="BV19" s="5"/>
+      <c r="BW19" s="16"/>
       <c r="BX19" s="5"/>
-      <c r="BY19" s="11"/>
-      <c r="BZ19" s="12"/>
-      <c r="CA19" s="12"/>
-      <c r="CB19" s="12"/>
-      <c r="CC19" s="12"/>
-      <c r="CD19" s="12"/>
-      <c r="CE19" s="12"/>
-      <c r="CF19" s="12"/>
-      <c r="CG19" s="12"/>
-      <c r="CH19" s="12"/>
-      <c r="CI19" s="12"/>
-      <c r="CJ19" s="12"/>
-      <c r="CK19" s="12"/>
-      <c r="CL19" s="12"/>
-      <c r="CM19" s="12"/>
-      <c r="CN19" s="12"/>
-      <c r="CO19" s="12"/>
-      <c r="CP19" s="18"/>
+      <c r="BY19" s="15"/>
+      <c r="BZ19" s="5"/>
+      <c r="CA19" s="5"/>
+      <c r="CB19" s="5"/>
+      <c r="CC19" s="5"/>
+      <c r="CD19" s="5"/>
+      <c r="CE19" s="5"/>
+      <c r="CF19" s="5"/>
+      <c r="CG19" s="5"/>
+      <c r="CH19" s="5"/>
+      <c r="CI19" s="5"/>
+      <c r="CJ19" s="5"/>
+      <c r="CK19" s="5"/>
+      <c r="CL19" s="5"/>
+      <c r="CM19" s="5"/>
+      <c r="CN19" s="5"/>
+      <c r="CO19" s="5"/>
+      <c r="CP19" s="17"/>
     </row>
     <row r="20" spans="7:94" x14ac:dyDescent="0.2">
       <c r="G20" s="6"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="5"/>
-      <c r="O20" s="5"/>
-      <c r="P20" s="5"/>
-      <c r="Q20" s="5"/>
-      <c r="R20" s="5"/>
-      <c r="S20" s="5"/>
-      <c r="T20" s="5"/>
-      <c r="U20" s="5"/>
-      <c r="V20" s="5"/>
-      <c r="W20" s="5"/>
-      <c r="X20" s="5"/>
-      <c r="Y20" s="5"/>
-      <c r="Z20" s="5"/>
-      <c r="AA20" s="5"/>
-      <c r="AB20" s="5"/>
-      <c r="AC20" s="5"/>
-      <c r="AD20" s="5"/>
-      <c r="AE20" s="17"/>
+      <c r="H20" s="8">
+        <v>4</v>
+      </c>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="9"/>
+      <c r="Q20" s="9"/>
+      <c r="R20" s="9"/>
+      <c r="S20" s="9"/>
+      <c r="T20" s="9"/>
+      <c r="U20" s="9"/>
+      <c r="V20" s="9"/>
+      <c r="W20" s="9"/>
+      <c r="X20" s="9"/>
+      <c r="Y20" s="9"/>
+      <c r="Z20" s="9"/>
+      <c r="AA20" s="9"/>
+      <c r="AB20" s="9"/>
+      <c r="AC20" s="9"/>
+      <c r="AD20" s="9"/>
+      <c r="AE20" s="14">
+        <v>5</v>
+      </c>
       <c r="AF20" s="7"/>
       <c r="AG20" s="5"/>
       <c r="AH20" s="5"/>
       <c r="AI20" s="5"/>
       <c r="AJ20" s="5"/>
       <c r="AK20" s="6"/>
-      <c r="AL20" s="15"/>
-      <c r="AM20" s="5"/>
-      <c r="AN20" s="5"/>
-      <c r="AO20" s="5"/>
-      <c r="AP20" s="5"/>
-      <c r="AQ20" s="5"/>
-      <c r="AR20" s="5"/>
-      <c r="AS20" s="5"/>
-      <c r="AT20" s="5"/>
-      <c r="AU20" s="5"/>
-      <c r="AV20" s="5"/>
-      <c r="AW20" s="5"/>
-      <c r="AX20" s="5"/>
-      <c r="AY20" s="5"/>
-      <c r="AZ20" s="5"/>
-      <c r="BA20" s="5"/>
-      <c r="BB20" s="5"/>
-      <c r="BC20" s="5"/>
-      <c r="BD20" s="5"/>
-      <c r="BE20" s="5"/>
-      <c r="BF20" s="5"/>
-      <c r="BG20" s="5"/>
-      <c r="BH20" s="5"/>
-      <c r="BI20" s="17"/>
+      <c r="AL20" s="8">
+        <v>4</v>
+      </c>
+      <c r="AM20" s="9"/>
+      <c r="AN20" s="9"/>
+      <c r="AO20" s="9"/>
+      <c r="AP20" s="9"/>
+      <c r="AQ20" s="9"/>
+      <c r="AR20" s="9"/>
+      <c r="AS20" s="9"/>
+      <c r="AT20" s="9"/>
+      <c r="AU20" s="9"/>
+      <c r="AV20" s="9"/>
+      <c r="AW20" s="9"/>
+      <c r="AX20" s="9"/>
+      <c r="AY20" s="9"/>
+      <c r="AZ20" s="9"/>
+      <c r="BA20" s="9"/>
+      <c r="BB20" s="9"/>
+      <c r="BC20" s="9"/>
+      <c r="BD20" s="9"/>
+      <c r="BE20" s="9"/>
+      <c r="BF20" s="9"/>
+      <c r="BG20" s="9"/>
+      <c r="BH20" s="9"/>
+      <c r="BI20" s="14">
+        <v>5</v>
+      </c>
       <c r="BJ20" s="7"/>
+      <c r="BS20" s="11"/>
+      <c r="BT20" s="12"/>
+      <c r="BU20" s="12"/>
+      <c r="BV20" s="12"/>
+      <c r="BW20" s="13"/>
+      <c r="BX20" s="5"/>
+      <c r="BY20" s="11"/>
+      <c r="BZ20" s="12"/>
+      <c r="CA20" s="12"/>
+      <c r="CB20" s="12"/>
+      <c r="CC20" s="12"/>
+      <c r="CD20" s="12"/>
+      <c r="CE20" s="12"/>
+      <c r="CF20" s="12"/>
+      <c r="CG20" s="12"/>
+      <c r="CH20" s="12"/>
+      <c r="CI20" s="12"/>
+      <c r="CJ20" s="12"/>
+      <c r="CK20" s="12"/>
+      <c r="CL20" s="12"/>
+      <c r="CM20" s="12"/>
+      <c r="CN20" s="12"/>
+      <c r="CO20" s="12"/>
+      <c r="CP20" s="18"/>
     </row>
     <row r="21" spans="7:94" x14ac:dyDescent="0.2">
       <c r="G21" s="6"/>
@@ -3865,7 +3911,7 @@
       <c r="AB22" s="5"/>
       <c r="AC22" s="5"/>
       <c r="AD22" s="5"/>
-      <c r="AE22" s="19"/>
+      <c r="AE22" s="17"/>
       <c r="AF22" s="7"/>
       <c r="AG22" s="5"/>
       <c r="AH22" s="5"/>
@@ -3900,30 +3946,30 @@
     </row>
     <row r="23" spans="7:94" x14ac:dyDescent="0.2">
       <c r="G23" s="6"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="12"/>
-      <c r="K23" s="12"/>
-      <c r="L23" s="12"/>
-      <c r="M23" s="12"/>
-      <c r="N23" s="12"/>
-      <c r="O23" s="12"/>
-      <c r="P23" s="12"/>
-      <c r="Q23" s="12"/>
-      <c r="R23" s="12"/>
-      <c r="S23" s="12"/>
-      <c r="T23" s="12"/>
-      <c r="U23" s="12"/>
-      <c r="V23" s="12"/>
-      <c r="W23" s="12"/>
-      <c r="X23" s="12"/>
-      <c r="Y23" s="12"/>
-      <c r="Z23" s="12"/>
-      <c r="AA23" s="12"/>
-      <c r="AB23" s="12"/>
-      <c r="AC23" s="12"/>
-      <c r="AD23" s="12"/>
-      <c r="AE23" s="18"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+      <c r="P23" s="5"/>
+      <c r="Q23" s="5"/>
+      <c r="R23" s="5"/>
+      <c r="S23" s="5"/>
+      <c r="T23" s="5"/>
+      <c r="U23" s="5"/>
+      <c r="V23" s="5"/>
+      <c r="W23" s="5"/>
+      <c r="X23" s="5"/>
+      <c r="Y23" s="5"/>
+      <c r="Z23" s="5"/>
+      <c r="AA23" s="5"/>
+      <c r="AB23" s="5"/>
+      <c r="AC23" s="5"/>
+      <c r="AD23" s="5"/>
+      <c r="AE23" s="19"/>
       <c r="AF23" s="7"/>
       <c r="AG23" s="5"/>
       <c r="AH23" s="5"/>
@@ -3956,33 +4002,33 @@
       <c r="BI23" s="17"/>
       <c r="BJ23" s="7"/>
     </row>
-    <row r="24" spans="7:94" ht="13.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G24" s="20"/>
-      <c r="H24" s="21"/>
-      <c r="I24" s="21"/>
-      <c r="J24" s="21"/>
-      <c r="K24" s="21"/>
-      <c r="L24" s="21"/>
-      <c r="M24" s="21"/>
-      <c r="N24" s="21"/>
-      <c r="O24" s="21"/>
-      <c r="P24" s="21"/>
-      <c r="Q24" s="21"/>
-      <c r="R24" s="21"/>
-      <c r="S24" s="21"/>
-      <c r="T24" s="21"/>
-      <c r="U24" s="21"/>
-      <c r="V24" s="21"/>
-      <c r="W24" s="21"/>
-      <c r="X24" s="21"/>
-      <c r="Y24" s="21"/>
-      <c r="Z24" s="21"/>
-      <c r="AA24" s="21"/>
-      <c r="AB24" s="21"/>
-      <c r="AC24" s="21"/>
-      <c r="AD24" s="21"/>
-      <c r="AE24" s="21"/>
-      <c r="AF24" s="22"/>
+    <row r="24" spans="7:94" x14ac:dyDescent="0.2">
+      <c r="G24" s="6"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="12"/>
+      <c r="N24" s="12"/>
+      <c r="O24" s="12"/>
+      <c r="P24" s="12"/>
+      <c r="Q24" s="12"/>
+      <c r="R24" s="12"/>
+      <c r="S24" s="12"/>
+      <c r="T24" s="12"/>
+      <c r="U24" s="12"/>
+      <c r="V24" s="12"/>
+      <c r="W24" s="12"/>
+      <c r="X24" s="12"/>
+      <c r="Y24" s="12"/>
+      <c r="Z24" s="12"/>
+      <c r="AA24" s="12"/>
+      <c r="AB24" s="12"/>
+      <c r="AC24" s="12"/>
+      <c r="AD24" s="12"/>
+      <c r="AE24" s="18"/>
+      <c r="AF24" s="7"/>
       <c r="AG24" s="5"/>
       <c r="AH24" s="5"/>
       <c r="AI24" s="5"/>
@@ -4014,33 +4060,33 @@
       <c r="BI24" s="17"/>
       <c r="BJ24" s="7"/>
     </row>
-    <row r="25" spans="7:94" x14ac:dyDescent="0.2">
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="5"/>
-      <c r="L25" s="5"/>
-      <c r="M25" s="5"/>
-      <c r="N25" s="5"/>
-      <c r="O25" s="5"/>
-      <c r="P25" s="5"/>
-      <c r="Q25" s="5"/>
-      <c r="R25" s="5"/>
-      <c r="S25" s="5"/>
-      <c r="T25" s="5"/>
-      <c r="U25" s="5"/>
-      <c r="V25" s="5"/>
-      <c r="W25" s="5"/>
-      <c r="X25" s="5"/>
-      <c r="Y25" s="5"/>
-      <c r="Z25" s="5"/>
-      <c r="AA25" s="5"/>
-      <c r="AB25" s="5"/>
-      <c r="AC25" s="5"/>
-      <c r="AD25" s="5"/>
-      <c r="AE25" s="5"/>
-      <c r="AF25" s="5"/>
+    <row r="25" spans="7:94" ht="13.8" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G25" s="20"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="21"/>
+      <c r="K25" s="21"/>
+      <c r="L25" s="21"/>
+      <c r="M25" s="21"/>
+      <c r="N25" s="21"/>
+      <c r="O25" s="21"/>
+      <c r="P25" s="21"/>
+      <c r="Q25" s="21"/>
+      <c r="R25" s="21"/>
+      <c r="S25" s="21"/>
+      <c r="T25" s="21"/>
+      <c r="U25" s="21"/>
+      <c r="V25" s="21"/>
+      <c r="W25" s="21"/>
+      <c r="X25" s="21"/>
+      <c r="Y25" s="21"/>
+      <c r="Z25" s="21"/>
+      <c r="AA25" s="21"/>
+      <c r="AB25" s="21"/>
+      <c r="AC25" s="21"/>
+      <c r="AD25" s="21"/>
+      <c r="AE25" s="21"/>
+      <c r="AF25" s="22"/>
       <c r="AG25" s="5"/>
       <c r="AH25" s="5"/>
       <c r="AI25" s="5"/>
@@ -4072,17 +4118,16 @@
       <c r="BI25" s="17"/>
       <c r="BJ25" s="7"/>
     </row>
-    <row r="26" spans="7:94" ht="23.4" x14ac:dyDescent="0.2">
+    <row r="26" spans="7:94" x14ac:dyDescent="0.2">
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
       <c r="L26" s="5"/>
       <c r="M26" s="5"/>
       <c r="N26" s="5"/>
-      <c r="O26" s="23" t="s">
-        <v>5</v>
-      </c>
+      <c r="O26" s="5"/>
       <c r="P26" s="5"/>
       <c r="Q26" s="5"/>
       <c r="R26" s="5"/>
@@ -4130,20 +4175,18 @@
       <c r="BH26" s="5"/>
       <c r="BI26" s="17"/>
       <c r="BJ26" s="7"/>
-      <c r="BN26" s="36" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="27" spans="7:94" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="7:94" ht="23.4" x14ac:dyDescent="0.2">
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
-      <c r="K27" s="5"/>
       <c r="L27" s="5"/>
       <c r="M27" s="5"/>
       <c r="N27" s="5"/>
-      <c r="O27" s="5"/>
+      <c r="O27" s="23" t="s">
+        <v>5</v>
+      </c>
       <c r="P27" s="5"/>
       <c r="Q27" s="5"/>
       <c r="R27" s="5"/>
@@ -4191,6 +4234,9 @@
       <c r="BH27" s="5"/>
       <c r="BI27" s="17"/>
       <c r="BJ27" s="7"/>
+      <c r="BN27" s="36" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="28" spans="7:94" x14ac:dyDescent="0.2">
       <c r="G28" s="5"/>
@@ -4421,7 +4467,7 @@
       <c r="BF31" s="5"/>
       <c r="BG31" s="5"/>
       <c r="BH31" s="5"/>
-      <c r="BI31" s="19"/>
+      <c r="BI31" s="17"/>
       <c r="BJ31" s="7"/>
     </row>
     <row r="32" spans="7:94" x14ac:dyDescent="0.2">
@@ -4514,33 +4560,33 @@
       <c r="AI33" s="5"/>
       <c r="AJ33" s="5"/>
       <c r="AK33" s="6"/>
-      <c r="AL33" s="11"/>
-      <c r="AM33" s="12"/>
-      <c r="AN33" s="12"/>
-      <c r="AO33" s="12"/>
-      <c r="AP33" s="12"/>
-      <c r="AQ33" s="12"/>
-      <c r="AR33" s="12"/>
-      <c r="AS33" s="12"/>
-      <c r="AT33" s="12"/>
-      <c r="AU33" s="12"/>
-      <c r="AV33" s="12"/>
-      <c r="AW33" s="12"/>
-      <c r="AX33" s="12"/>
-      <c r="AY33" s="12"/>
-      <c r="AZ33" s="12"/>
-      <c r="BA33" s="12"/>
-      <c r="BB33" s="12"/>
-      <c r="BC33" s="12"/>
-      <c r="BD33" s="12"/>
-      <c r="BE33" s="12"/>
-      <c r="BF33" s="12"/>
-      <c r="BG33" s="12"/>
-      <c r="BH33" s="12"/>
-      <c r="BI33" s="18"/>
+      <c r="AL33" s="15"/>
+      <c r="AM33" s="5"/>
+      <c r="AN33" s="5"/>
+      <c r="AO33" s="5"/>
+      <c r="AP33" s="5"/>
+      <c r="AQ33" s="5"/>
+      <c r="AR33" s="5"/>
+      <c r="AS33" s="5"/>
+      <c r="AT33" s="5"/>
+      <c r="AU33" s="5"/>
+      <c r="AV33" s="5"/>
+      <c r="AW33" s="5"/>
+      <c r="AX33" s="5"/>
+      <c r="AY33" s="5"/>
+      <c r="AZ33" s="5"/>
+      <c r="BA33" s="5"/>
+      <c r="BB33" s="5"/>
+      <c r="BC33" s="5"/>
+      <c r="BD33" s="5"/>
+      <c r="BE33" s="5"/>
+      <c r="BF33" s="5"/>
+      <c r="BG33" s="5"/>
+      <c r="BH33" s="5"/>
+      <c r="BI33" s="19"/>
       <c r="BJ33" s="7"/>
     </row>
-    <row r="34" spans="6:80" ht="13.8" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="6:80" x14ac:dyDescent="0.2">
       <c r="G34" s="5"/>
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
@@ -4571,34 +4617,34 @@
       <c r="AH34" s="5"/>
       <c r="AI34" s="5"/>
       <c r="AJ34" s="5"/>
-      <c r="AK34" s="20"/>
-      <c r="AL34" s="21"/>
-      <c r="AM34" s="21"/>
-      <c r="AN34" s="21"/>
-      <c r="AO34" s="21"/>
-      <c r="AP34" s="21"/>
-      <c r="AQ34" s="21"/>
-      <c r="AR34" s="21"/>
-      <c r="AS34" s="21"/>
-      <c r="AT34" s="21"/>
-      <c r="AU34" s="21"/>
-      <c r="AV34" s="21"/>
-      <c r="AW34" s="21"/>
-      <c r="AX34" s="21"/>
-      <c r="AY34" s="21"/>
-      <c r="AZ34" s="21"/>
-      <c r="BA34" s="21"/>
-      <c r="BB34" s="21"/>
-      <c r="BC34" s="21"/>
-      <c r="BD34" s="21"/>
-      <c r="BE34" s="21"/>
-      <c r="BF34" s="21"/>
-      <c r="BG34" s="21"/>
-      <c r="BH34" s="21"/>
-      <c r="BI34" s="21"/>
-      <c r="BJ34" s="22"/>
-    </row>
-    <row r="35" spans="6:80" x14ac:dyDescent="0.2">
+      <c r="AK34" s="6"/>
+      <c r="AL34" s="11"/>
+      <c r="AM34" s="12"/>
+      <c r="AN34" s="12"/>
+      <c r="AO34" s="12"/>
+      <c r="AP34" s="12"/>
+      <c r="AQ34" s="12"/>
+      <c r="AR34" s="12"/>
+      <c r="AS34" s="12"/>
+      <c r="AT34" s="12"/>
+      <c r="AU34" s="12"/>
+      <c r="AV34" s="12"/>
+      <c r="AW34" s="12"/>
+      <c r="AX34" s="12"/>
+      <c r="AY34" s="12"/>
+      <c r="AZ34" s="12"/>
+      <c r="BA34" s="12"/>
+      <c r="BB34" s="12"/>
+      <c r="BC34" s="12"/>
+      <c r="BD34" s="12"/>
+      <c r="BE34" s="12"/>
+      <c r="BF34" s="12"/>
+      <c r="BG34" s="12"/>
+      <c r="BH34" s="12"/>
+      <c r="BI34" s="18"/>
+      <c r="BJ34" s="7"/>
+    </row>
+    <row r="35" spans="6:80" ht="13.8" thickBot="1" x14ac:dyDescent="0.25">
       <c r="G35" s="5"/>
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
@@ -4629,12 +4675,34 @@
       <c r="AH35" s="5"/>
       <c r="AI35" s="5"/>
       <c r="AJ35" s="5"/>
-      <c r="AK35" s="5"/>
-      <c r="AL35" s="5"/>
-      <c r="AM35" s="5"/>
-      <c r="AN35" s="5"/>
-    </row>
-    <row r="36" spans="6:80" ht="28.2" x14ac:dyDescent="0.2">
+      <c r="AK35" s="20"/>
+      <c r="AL35" s="21"/>
+      <c r="AM35" s="21"/>
+      <c r="AN35" s="21"/>
+      <c r="AO35" s="21"/>
+      <c r="AP35" s="21"/>
+      <c r="AQ35" s="21"/>
+      <c r="AR35" s="21"/>
+      <c r="AS35" s="21"/>
+      <c r="AT35" s="21"/>
+      <c r="AU35" s="21"/>
+      <c r="AV35" s="21"/>
+      <c r="AW35" s="21"/>
+      <c r="AX35" s="21"/>
+      <c r="AY35" s="21"/>
+      <c r="AZ35" s="21"/>
+      <c r="BA35" s="21"/>
+      <c r="BB35" s="21"/>
+      <c r="BC35" s="21"/>
+      <c r="BD35" s="21"/>
+      <c r="BE35" s="21"/>
+      <c r="BF35" s="21"/>
+      <c r="BG35" s="21"/>
+      <c r="BH35" s="21"/>
+      <c r="BI35" s="21"/>
+      <c r="BJ35" s="22"/>
+    </row>
+    <row r="36" spans="6:80" x14ac:dyDescent="0.2">
       <c r="G36" s="5"/>
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
@@ -4669,11 +4737,8 @@
       <c r="AL36" s="5"/>
       <c r="AM36" s="5"/>
       <c r="AN36" s="5"/>
-      <c r="AS36" s="24" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="6:80" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="6:80" ht="28.2" x14ac:dyDescent="0.2">
       <c r="G37" s="5"/>
       <c r="H37" s="5"/>
       <c r="I37" s="5"/>
@@ -4708,6 +4773,9 @@
       <c r="AL37" s="5"/>
       <c r="AM37" s="5"/>
       <c r="AN37" s="5"/>
+      <c r="AS37" s="24" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="38" spans="6:80" x14ac:dyDescent="0.2">
       <c r="G38" s="5"/>
@@ -4745,10 +4813,8 @@
       <c r="AM38" s="5"/>
       <c r="AN38" s="5"/>
     </row>
-    <row r="39" spans="6:80" ht="19.2" x14ac:dyDescent="0.2">
-      <c r="F39" s="25" t="s">
-        <v>7</v>
-      </c>
+    <row r="39" spans="6:80" x14ac:dyDescent="0.2">
+      <c r="G39" s="5"/>
       <c r="H39" s="5"/>
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
@@ -4779,14 +4845,13 @@
       <c r="AI39" s="5"/>
       <c r="AJ39" s="5"/>
       <c r="AK39" s="5"/>
-      <c r="AL39" s="26"/>
+      <c r="AL39" s="5"/>
       <c r="AM39" s="5"/>
       <c r="AN39" s="5"/>
-      <c r="CA39" s="25"/>
     </row>
     <row r="40" spans="6:80" ht="19.2" x14ac:dyDescent="0.2">
-      <c r="G40" s="27" t="s">
-        <v>8</v>
+      <c r="F40" s="25" t="s">
+        <v>7</v>
       </c>
       <c r="H40" s="5"/>
       <c r="I40" s="5"/>
@@ -4818,14 +4883,14 @@
       <c r="AI40" s="5"/>
       <c r="AJ40" s="5"/>
       <c r="AK40" s="5"/>
-      <c r="AL40" s="5"/>
+      <c r="AL40" s="26"/>
       <c r="AM40" s="5"/>
-      <c r="AN40" s="28"/>
-      <c r="CB40" s="28"/>
+      <c r="AN40" s="5"/>
+      <c r="CA40" s="25"/>
     </row>
     <row r="41" spans="6:80" ht="19.2" x14ac:dyDescent="0.2">
       <c r="G41" s="27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H41" s="5"/>
       <c r="I41" s="5"/>
@@ -4859,12 +4924,12 @@
       <c r="AK41" s="5"/>
       <c r="AL41" s="5"/>
       <c r="AM41" s="5"/>
-      <c r="AN41" s="29"/>
-      <c r="CB41" s="30"/>
+      <c r="AN41" s="28"/>
+      <c r="CB41" s="28"/>
     </row>
     <row r="42" spans="6:80" ht="19.2" x14ac:dyDescent="0.2">
       <c r="G42" s="27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H42" s="5"/>
       <c r="I42" s="5"/>
@@ -4903,7 +4968,7 @@
     </row>
     <row r="43" spans="6:80" ht="19.2" x14ac:dyDescent="0.2">
       <c r="G43" s="27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H43" s="5"/>
       <c r="I43" s="5"/>
@@ -4942,7 +5007,7 @@
     </row>
     <row r="44" spans="6:80" ht="19.2" x14ac:dyDescent="0.2">
       <c r="G44" s="27" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H44" s="5"/>
       <c r="I44" s="5"/>
@@ -4976,12 +5041,12 @@
       <c r="AK44" s="5"/>
       <c r="AL44" s="5"/>
       <c r="AM44" s="5"/>
-      <c r="AN44" s="28"/>
+      <c r="AN44" s="29"/>
       <c r="CB44" s="30"/>
     </row>
     <row r="45" spans="6:80" ht="19.2" x14ac:dyDescent="0.2">
       <c r="G45" s="27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H45" s="5"/>
       <c r="I45" s="5"/>
@@ -5015,11 +5080,13 @@
       <c r="AK45" s="5"/>
       <c r="AL45" s="5"/>
       <c r="AM45" s="5"/>
-      <c r="AN45" s="29"/>
+      <c r="AN45" s="28"/>
       <c r="CB45" s="30"/>
     </row>
     <row r="46" spans="6:80" ht="19.2" x14ac:dyDescent="0.2">
-      <c r="G46" s="27"/>
+      <c r="G46" s="27" t="s">
+        <v>13</v>
+      </c>
       <c r="H46" s="5"/>
       <c r="I46" s="5"/>
       <c r="J46" s="5"/>
@@ -5052,16 +5119,50 @@
       <c r="AK46" s="5"/>
       <c r="AL46" s="5"/>
       <c r="AM46" s="5"/>
-      <c r="AN46" s="27"/>
+      <c r="AN46" s="29"/>
       <c r="CB46" s="30"/>
     </row>
     <row r="47" spans="6:80" ht="19.2" x14ac:dyDescent="0.2">
-      <c r="G47" s="28"/>
-      <c r="AN47" s="30"/>
+      <c r="G47" s="27"/>
+      <c r="H47" s="5"/>
+      <c r="I47" s="5"/>
+      <c r="J47" s="5"/>
+      <c r="K47" s="5"/>
+      <c r="L47" s="5"/>
+      <c r="M47" s="5"/>
+      <c r="N47" s="5"/>
+      <c r="O47" s="5"/>
+      <c r="P47" s="5"/>
+      <c r="Q47" s="5"/>
+      <c r="R47" s="5"/>
+      <c r="S47" s="5"/>
+      <c r="T47" s="5"/>
+      <c r="U47" s="5"/>
+      <c r="V47" s="5"/>
+      <c r="W47" s="5"/>
+      <c r="X47" s="5"/>
+      <c r="Y47" s="5"/>
+      <c r="Z47" s="5"/>
+      <c r="AA47" s="5"/>
+      <c r="AB47" s="5"/>
+      <c r="AC47" s="5"/>
+      <c r="AD47" s="5"/>
+      <c r="AE47" s="5"/>
+      <c r="AF47" s="5"/>
+      <c r="AG47" s="5"/>
+      <c r="AH47" s="5"/>
+      <c r="AI47" s="5"/>
+      <c r="AJ47" s="5"/>
+      <c r="AK47" s="5"/>
+      <c r="AL47" s="5"/>
+      <c r="AM47" s="5"/>
+      <c r="AN47" s="27"/>
       <c r="CB47" s="30"/>
     </row>
     <row r="48" spans="6:80" ht="19.2" x14ac:dyDescent="0.2">
       <c r="G48" s="28"/>
+      <c r="AN48" s="30"/>
+      <c r="CB48" s="30"/>
     </row>
     <row r="49" spans="7:7" ht="19.2" x14ac:dyDescent="0.2">
       <c r="G49" s="28"/>
@@ -5080,12 +5181,15 @@
     </row>
     <row r="54" spans="7:7" ht="19.2" x14ac:dyDescent="0.2">
       <c r="G54" s="28"/>
+    </row>
+    <row r="55" spans="7:7" ht="19.2" x14ac:dyDescent="0.2">
+      <c r="G55" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="AD8:AE9"/>
     <mergeCell ref="BH8:BI9"/>
-    <mergeCell ref="AL12:AP16"/>
+    <mergeCell ref="AL13:AP17"/>
     <mergeCell ref="AM8:AM9"/>
     <mergeCell ref="CO8:CP9"/>
   </mergeCells>
@@ -5115,63 +5219,63 @@
   <sheetData>
     <row r="3" spans="2:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B4" s="78" t="s">
+      <c r="B4" s="76" t="s">
+        <v>114</v>
+      </c>
+      <c r="C4" s="74"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="74"/>
+      <c r="F4" s="75"/>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B5" s="71"/>
+      <c r="C5" s="72"/>
+      <c r="D5" s="72"/>
+      <c r="E5" s="72"/>
+      <c r="F5" s="73"/>
+    </row>
+    <row r="6" spans="2:6" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="71"/>
+      <c r="C6" s="77" t="s">
+        <v>116</v>
+      </c>
+      <c r="D6" s="72" t="s">
         <v>115</v>
       </c>
-      <c r="C4" s="76"/>
-      <c r="D4" s="76"/>
-      <c r="E4" s="76"/>
-      <c r="F4" s="77"/>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B5" s="73"/>
-      <c r="C5" s="74"/>
-      <c r="D5" s="74"/>
-      <c r="E5" s="74"/>
-      <c r="F5" s="75"/>
-    </row>
-    <row r="6" spans="2:6" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="73"/>
-      <c r="C6" s="79" t="s">
-        <v>117</v>
-      </c>
-      <c r="D6" s="74" t="s">
-        <v>116</v>
-      </c>
-      <c r="E6" s="74"/>
-      <c r="F6" s="75"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="73"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B7" s="73"/>
-      <c r="C7" s="74"/>
-      <c r="D7" s="74"/>
-      <c r="E7" s="74"/>
-      <c r="F7" s="75"/>
+      <c r="B7" s="71"/>
+      <c r="C7" s="72"/>
+      <c r="D7" s="72"/>
+      <c r="E7" s="72"/>
+      <c r="F7" s="73"/>
     </row>
     <row r="8" spans="2:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="95" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C8" s="96"/>
       <c r="D8" s="97"/>
       <c r="E8" s="98" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F8" s="99"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B9" s="74"/>
-      <c r="C9" s="74"/>
-      <c r="D9" s="74"/>
-      <c r="E9" s="74"/>
-      <c r="F9" s="74"/>
+      <c r="B9" s="72"/>
+      <c r="C9" s="72"/>
+      <c r="D9" s="72"/>
+      <c r="E9" s="72"/>
+      <c r="F9" s="72"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B10" s="74"/>
-      <c r="C10" s="74"/>
-      <c r="D10" s="74"/>
-      <c r="E10" s="74"/>
-      <c r="F10" s="74"/>
+      <c r="B10" s="72"/>
+      <c r="C10" s="72"/>
+      <c r="D10" s="72"/>
+      <c r="E10" s="72"/>
+      <c r="F10" s="72"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -5358,10 +5462,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:C34"/>
+  <dimension ref="B1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -5436,7 +5540,7 @@
       </c>
     </row>
     <row r="10" spans="2:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="67" t="s">
+      <c r="B10" s="65" t="s">
         <v>44</v>
       </c>
       <c r="C10" s="35" t="s">
@@ -5561,57 +5665,79 @@
     </row>
     <row r="27" spans="2:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="101" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C27" s="35" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="28" spans="2:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="102"/>
       <c r="C28" s="35" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29" spans="2:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="72"/>
+      <c r="B29" s="70"/>
       <c r="C29" s="35" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="30" spans="2:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="103" t="s">
+      <c r="B30" s="78" t="s">
+        <v>121</v>
+      </c>
+      <c r="C30" s="35" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="78" t="s">
+        <v>123</v>
+      </c>
+      <c r="C31" s="35" t="s">
         <v>122</v>
       </c>
-      <c r="C30" s="35" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="103" t="s">
+    </row>
+    <row r="32" spans="2:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="78" t="s">
+        <v>120</v>
+      </c>
+      <c r="C32" s="35" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="104"/>
+      <c r="C33" s="105" t="s">
         <v>124</v>
       </c>
-      <c r="C31" s="35" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="103" t="s">
-        <v>121</v>
-      </c>
-      <c r="C32" s="35" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="68"/>
-      <c r="C33" s="35" t="s">
+    </row>
+    <row r="34" spans="2:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="70" t="s">
+        <v>126</v>
+      </c>
+      <c r="C34" s="103" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="34" spans="2:3" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="45"/>
-      <c r="C34" s="104"/>
+    <row r="35" spans="2:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="66"/>
+      <c r="C35" s="103" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="66" t="s">
+        <v>129</v>
+      </c>
+      <c r="C36" s="103" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="45"/>
+      <c r="C37" s="79"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -5633,9 +5759,10 @@
     <hyperlink ref="C18" r:id="rId11"/>
     <hyperlink ref="C20" r:id="rId12"/>
     <hyperlink ref="C19" r:id="rId13" location="attr_android:imeOptions"/>
+    <hyperlink ref="C35" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
 

</xml_diff>